<commit_message>
added lowes quarterly data
</commit_message>
<xml_diff>
--- a/data_files/additional_data/low_revenue.xlsx
+++ b/data_files/additional_data/low_revenue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Documents/Data_Science/Time_Series/time-series-examples/additional_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Documents/Data_Science/Time_Series/time-series-examples/data_files/additional_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A4DAF58-EF2A-3641-841A-DF75C492A562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC9180B-48DD-A041-8FBE-C8C682E8354F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="24960" windowHeight="15900" xr2:uid="{6A154736-59B1-9C4B-92E9-D407BF21640E}"/>
+    <workbookView xWindow="18740" yWindow="460" windowWidth="24960" windowHeight="15900" xr2:uid="{6A154736-59B1-9C4B-92E9-D407BF21640E}"/>
   </bookViews>
   <sheets>
     <sheet name="low_revenue" sheetId="1" r:id="rId1"/>
@@ -397,11 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2109A32B-8125-3849-B0B1-5CD9F5A699FF}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -532,122 +530,306 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>42769</v>
+        <v>40662</v>
       </c>
       <c r="B16" s="1">
-        <v>15784</v>
+        <v>12185</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>42857</v>
+        <v>40753</v>
       </c>
       <c r="B17" s="1">
-        <v>16860</v>
+        <v>14543</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>42949</v>
+        <v>40844</v>
       </c>
       <c r="B18" s="1">
-        <v>19495</v>
+        <v>11852</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>43041</v>
+        <v>40942</v>
       </c>
       <c r="B19" s="1">
-        <v>16770</v>
+        <v>11629</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>43133</v>
+        <v>41033</v>
       </c>
       <c r="B20" s="1">
-        <v>15494</v>
+        <v>13153</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>43222</v>
+        <v>41124</v>
       </c>
       <c r="B21" s="1">
-        <v>17360</v>
+        <v>14249</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>43314</v>
+        <v>41215</v>
       </c>
       <c r="B22" s="1">
-        <v>20888</v>
+        <v>12073</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>43406</v>
+        <v>41306</v>
       </c>
       <c r="B23" s="1">
-        <v>17415</v>
+        <v>11046</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>43497</v>
+        <v>41397</v>
       </c>
       <c r="B24" s="1">
-        <v>15647</v>
+        <v>13088</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>43586</v>
+        <v>41488</v>
       </c>
       <c r="B25" s="1">
-        <v>17741</v>
+        <v>15711</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>43678</v>
+        <v>41579</v>
       </c>
       <c r="B26" s="1">
-        <v>20992</v>
+        <v>12957</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>43770</v>
+        <v>41670</v>
       </c>
       <c r="B27" s="1">
-        <v>17388</v>
+        <v>11660</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>43861</v>
+        <v>41761</v>
       </c>
       <c r="B28" s="1">
-        <v>16027</v>
+        <v>13403</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>43951</v>
+        <v>41852</v>
       </c>
       <c r="B29" s="1">
-        <v>19675</v>
+        <v>16599</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
+        <v>41943</v>
+      </c>
+      <c r="B30" s="1">
+        <v>13681</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2">
+        <v>42034</v>
+      </c>
+      <c r="B31" s="1">
+        <v>12540</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
+        <v>42125</v>
+      </c>
+      <c r="B32" s="1">
+        <v>14129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
+        <v>42216</v>
+      </c>
+      <c r="B33" s="1">
+        <v>17348</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2">
+        <v>42307</v>
+      </c>
+      <c r="B34" s="1">
+        <v>14360</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B35" s="1">
+        <v>13236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2">
+        <v>42489</v>
+      </c>
+      <c r="B36" s="1">
+        <v>15234</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2">
+        <v>42580</v>
+      </c>
+      <c r="B37" s="1">
+        <v>18260</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2">
+        <v>42671</v>
+      </c>
+      <c r="B38" s="1">
+        <v>15739</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="2">
+        <v>42769</v>
+      </c>
+      <c r="B39" s="1">
+        <v>15784</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2">
+        <v>42857</v>
+      </c>
+      <c r="B40" s="1">
+        <v>16860</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2">
+        <v>42949</v>
+      </c>
+      <c r="B41" s="1">
+        <v>19495</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="2">
+        <v>43041</v>
+      </c>
+      <c r="B42" s="1">
+        <v>16770</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="2">
+        <v>43133</v>
+      </c>
+      <c r="B43" s="1">
+        <v>15494</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="2">
+        <v>43222</v>
+      </c>
+      <c r="B44" s="1">
+        <v>17360</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="2">
+        <v>43314</v>
+      </c>
+      <c r="B45" s="1">
+        <v>20888</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="2">
+        <v>43406</v>
+      </c>
+      <c r="B46" s="1">
+        <v>17415</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2">
+        <v>43497</v>
+      </c>
+      <c r="B47" s="1">
+        <v>15647</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2">
+        <v>43586</v>
+      </c>
+      <c r="B48" s="1">
+        <v>17741</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2">
+        <v>43678</v>
+      </c>
+      <c r="B49" s="1">
+        <v>20992</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2">
+        <v>43770</v>
+      </c>
+      <c r="B50" s="1">
+        <v>17388</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2">
+        <v>43861</v>
+      </c>
+      <c r="B51" s="1">
+        <v>16027</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B52" s="1">
+        <v>19675</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2">
         <v>44042</v>
       </c>
-      <c r="B30" s="1">
-        <v>27307</v>
+      <c r="B53" s="1">
+        <v>27302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>